<commit_message>
feat: Putri + Max added to factory system - all 25 models now have intensity meters and calibrated sexting
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/max/Max_Complete_Infloww.xlsx
+++ b/max/Max_Complete_Infloww.xlsx
@@ -8,41 +8,39 @@
   </bookViews>
   <sheets>
     <sheet name="MaxJourney" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MeetupRedirect" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NRWaves" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="PersonalMax" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PositiveSpin" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="LocationHandling" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ReEngagement" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="price1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="price2" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="discount1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="discount2" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="free1" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="free2" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="nomoney1" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="nomoney2" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="noppv1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="noppv2" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="card1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="card2" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="nosex1" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="nosex2" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="offtopic1" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="offtopic2" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="real1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="real2" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="voice1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="voice2" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="customyes1" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="customyes2" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="customno1" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="customno2" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="done1" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="done2" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="cumcontrol" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="dickpic" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="boosters" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="NRWaves" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PersonalMax" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PositiveSpin" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ReEngagement" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="price1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="price2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="discount1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="discount2" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="free1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="free2" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="nomoney1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="nomoney2" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="noppv1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="noppv2" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="card1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="card2" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="nosex1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="nosex2" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="offtopic1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="offtopic2" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="real1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="real2" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="voice1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="voice2" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="customyes1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="customyes2" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="customno1" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="customno2" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="done1" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="done2" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="cumcontrol1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="dickpic" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="boosters" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -81,49 +79,41 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4472C4"/>
-        <bgColor rgb="FF4472C4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD0E0E3"/>
-        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6B26B"/>
-        <bgColor rgb="FFF6B26B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0F7FA"/>
-        <bgColor rgb="FFE0F7FA"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D2E9"/>
-        <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
@@ -617,17 +607,17 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Mention something specific he said/did. Then KEEP TALKING — build bond, GFE. NEVER say goodbye.</t>
+          <t>Mention something specific he said. KEEP TALKING. Build bond. NEVER say goodbye.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Character limits
+          <t>Character limits
 Name: Up to 64 characters
 Tag: Up to 32 characters
 Text: Up to 1000 characters
 Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
+Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported.</t>
         </is>
       </c>
     </row>
@@ -642,7 +632,7 @@
           <t>holy fuck 🥵 that was insane</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n"/>
+      <c r="C3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -652,7 +642,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>cum with me 💦😈</t>
+          <t>cum with me... watch me cum 💦😈</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -686,10 +676,10 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>I wanna finish with you... I'm close</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="n"/>
+          <t>I wanna finish with you... my cock is throbbing so hard and I'm about to blow everywhere</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -699,10 +689,10 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>don't cum yet</t>
-        </is>
-      </c>
-      <c r="C7" s="6" t="n"/>
+          <t>don't cum yet... my cock is pulsing and I need you to wait for me</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -712,7 +702,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>FUCK 🥵🥵</t>
+          <t>FUCK my cock is throbbing so hard I can barely think 🥵🥵</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -734,7 +724,7 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>SEND PPV 3 — $40. Bought → continue. Silent 3 min → NR Waves.</t>
+          <t>SEND PPV 3 — $40. Bought → continue. Silent → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -763,10 +753,10 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>fuck I can't hold back anymore</t>
-        </is>
-      </c>
-      <c r="C11" s="6" t="n"/>
+          <t>fuck I can't hold back anymore... I'm about to cum so hard</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
@@ -779,7 +769,7 @@
           <t>imagine me pinning you down and making you take every inch while you're begging for more 🥵</t>
         </is>
       </c>
-      <c r="C12" s="5" t="n"/>
+      <c r="C12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
@@ -792,7 +782,7 @@
           <t>I need to cum so bad rn you have no idea</t>
         </is>
       </c>
-      <c r="C13" s="6" t="n"/>
+      <c r="C13" s="6" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
@@ -802,7 +792,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>🥵🥵</t>
+          <t>FUCK I'm throbbing so hard 🥵🥵</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
@@ -824,7 +814,7 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>SEND PPV 2 — $25. Bought → continue. Silent 3 min → NR Waves.</t>
+          <t>SEND PPV 2 — $25. Bought → continue. Silent → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -858,7 +848,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Wait for reply. React to what he says before continuing.</t>
+          <t>Wait for reply. After: react to what he said.</t>
         </is>
       </c>
     </row>
@@ -873,7 +863,7 @@
           <t>I'm hard as fuck because of you and I can't do anything about it</t>
         </is>
       </c>
-      <c r="C18" s="5" t="n"/>
+      <c r="C18" s="5" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -883,12 +873,12 @@
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
-          <t>fuck... talking to you is doing something to me rn 🥵</t>
+          <t>fuck... talking to you is doing something to me rn 🥵 I'm getting hard as fuck</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>React to what he said. HE caused this.</t>
+          <t>React to what he said — HE caused this.</t>
         </is>
       </c>
     </row>
@@ -922,7 +912,7 @@
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>SEND PPV 1 — $12. Bought → continue. Silent 3 min → NR Waves.</t>
+          <t>SEND PPV 1 — $12. Bought → continue. Silent → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -954,7 +944,7 @@
           <t>you wanna see more? I'm feeling generous rn</t>
         </is>
       </c>
-      <c r="C23" s="6" t="n"/>
+      <c r="C23" s="6" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
@@ -964,12 +954,12 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>knew you'd like it 😈</t>
+          <t>knew you'd like it 😈 that's making me hard already</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>Add a short react ('haha damn', 'oh yeah?', '🥵')</t>
+          <t>Add a short react ('haha damn', 'oh yeah?').</t>
         </is>
       </c>
     </row>
@@ -986,7 +976,7 @@
       </c>
       <c r="C25" s="6" t="inlineStr">
         <is>
-          <t>Wait for reply.</t>
+          <t>Wait for his reply.</t>
         </is>
       </c>
     </row>
@@ -1003,7 +993,7 @@
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>SEND PPV 0 — FREE teaser (shirtless/post-gym). Wait for reply. Silent 3 min → NR Waves.</t>
+          <t>SEND PPV 0 — FREE teaser (shirtless/gym shot). Wait for reply. Silent 3 min → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1027,7 @@
       </c>
       <c r="C28" s="7" t="inlineStr">
         <is>
-          <t>If sexual reply → add 'especially after what you just said' before 'you're'</t>
+          <t>If he said something sexual → add 'especially after what you just said'.</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1061,7 @@
       </c>
       <c r="C30" s="7" t="inlineStr">
         <is>
-          <t>THE PIVOT. Physical context.</t>
+          <t>THE PIVOT — physical context: just trained, body activated.</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1078,7 @@
       </c>
       <c r="C31" s="8" t="inlineStr">
         <is>
-          <t>Ego boost. Next → TB-1. From MR path: go TB-1 + TB-2 then skip to S1-1.</t>
+          <t>Ego boost. Transition to TB-1.</t>
         </is>
       </c>
     </row>
@@ -1103,7 +1093,7 @@
           <t>so what do you do besides making me check my phone every 5 seconds 😏</t>
         </is>
       </c>
-      <c r="C32" s="8" t="n"/>
+      <c r="C32" s="8" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="8" t="inlineStr">
@@ -1118,7 +1108,7 @@
       </c>
       <c r="C33" s="8" t="inlineStr">
         <is>
-          <t>If he named somewhere Max visited → add 'oh I've been there' before 'nice'</t>
+          <t>If he named somewhere Max visited → add 'oh I've been there'.</t>
         </is>
       </c>
     </row>
@@ -1135,7 +1125,7 @@
       </c>
       <c r="C34" s="8" t="inlineStr">
         <is>
-          <t>Add a short react before ('haha damn', 'I like that', 'oh word?')</t>
+          <t>Add a short react ('haha damn', 'I like that', 'oh word?').</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1142,7 @@
       </c>
       <c r="C35" s="8" t="inlineStr">
         <is>
-          <t>Add his name before 'man'</t>
+          <t>Add his name before 'man'.</t>
         </is>
       </c>
     </row>
@@ -1206,38 +1196,38 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Takeaway</t>
+          <t>Step4 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>if you don't want it that's cool, I'll keep it for myself... or maybe someone else has been asking</t>
+          <t>it's cool, I'm not going anywhere... let's just keep talking, I like this</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>TAKEAWAY. Jealousy. Final step.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Concession</t>
+          <t>Step3 Guilt</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>alright... [lower price] just for you but don't tell anyone, this stays between us</t>
+          <t>I literally just recorded this because of what YOU said to me, this wasn't just random content man</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>CONCESSION. ONE TIME. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>GUILT. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
@@ -1247,33 +1237,33 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>I don't do discounts... I only share this with guys who actually appreciate what they're getting</t>
+          <t>free? nah I don't just give this to anyone... you gotta earn the good stuff</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Worthiness. Still pushing -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Firmness</t>
+          <t>Step1 Reminder</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>haha you trying to negotiate with me? this isn't a negotiation man, it's worth every cent</t>
+          <t>I already sent you one for free remember? and this one is way crazier... you have no idea</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>FIRMNESS. Playful. Still pushing -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>REMINDER. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1325,38 +1315,38 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Takeaway</t>
+          <t>Step4 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>alright I'll save it for someone who actually wants it then</t>
+          <t>no pressure at all, I'm just enjoying talking to you honestly</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>TAKEAWAY. Final.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Concession</t>
+          <t>Step3 Guilt</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>fine... [lower price] but ONLY because I like you, one time thing</t>
+          <t>I did this because of you... like specifically because of our convo, that took effort and I did it for YOU</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>CONCESSION. ONE TIME. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>GUILT. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
@@ -1366,33 +1356,33 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>the guys who appreciate what I do don't ask for discounts, just saying</t>
+          <t>free? you think the best things in life are free? not this one</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Still pushing -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Firmness</t>
+          <t>Step1 Reminder</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>a discount? do I look like I'm on sale?</t>
+          <t>you already got a free one, this one is on another level trust me</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>FIRMNESS. Short + confident. Still pushing -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>REMINDER. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1444,74 +1434,74 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Seed</t>
+          <t>Step4 Protect</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>it's cool, I'm not going anywhere... let's just keep talking, I like this</t>
+          <t>honestly it's fine, I like talking to you money or not... you do something to me</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>SEED. Protect relationship.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>PROTECT.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Guilt</t>
+          <t>Step3 PWYW</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>I literally just recorded this because of what YOU said to me, this wasn't just random content man</t>
+          <t>just send whatever you can man... even a tiny amount, I just need you to see what you made me do</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>GUILT. Reciprocity. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>PWYW. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>Step2 Test</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>free? nah I don't just give this to anyone... you gotta earn the good stuff</t>
+          <t>not even like [small amount]? I really want you to see this one</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Buying = earning. Still free -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>TEST $3-5. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reminder</t>
+          <t>Step1 Empathy</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>I already sent you one for free remember? and this one is way crazier... you have no idea</t>
+          <t>hey I totally get it, no pressure at all okay?</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>REMINDER. PPV0 was free. Still wants free -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>EMPATHY. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1563,74 +1553,74 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Seed</t>
+          <t>Step4 Protect</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>no pressure at all, I'm just enjoying talking to you honestly</t>
+          <t>it's totally cool, you being here is what matters</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>SEED.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>PROTECT.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Guilt</t>
+          <t>Step3 PWYW</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>I did this because of you... like specifically because of our convo, that took effort and I did it for YOU</t>
+          <t>send whatever feels right, even $1... I can't keep this from you</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>GUILT. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>PWYW. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>Step2 Test</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>free? you think the best things in life are free? not this one</t>
+          <t>what about just [small amount]? I really don't want you to miss this</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Still free -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>TEST. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reminder</t>
+          <t>Step1 Empathy</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>you already got a free one, this one is on another level trust me</t>
+          <t>that's fine, seriously don't worry about it</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>REMINDER. Still wants free -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>EMPATHY. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1643,7 +1633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1682,74 +1672,56 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Protect</t>
+          <t>Step3 PWYW</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>honestly it's fine, I like talking to you money or not... you do something to me</t>
+          <t>just send whatever you want, even $1, I can't keep this to myself... you need to see it</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>PROTECT. GFE. Tag for re-engagement.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>PWYW.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>Step2 Reframe</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>just send whatever you can man... even a tiny amount, I just need you to see what you made me do</t>
+          <t>look this isn't about money... I just need you to see what you're doing to me rn, I don't react like this to people</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>PAY WHAT YOU WANT. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>REFRAME. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Test</t>
+          <t>Step1 Accept</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>not even like [small amount]? I really want you to see this one</t>
+          <t>that's totally fine I'm not trying to sell you anything, I just like talking to you</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>TEST. Suggest $3-5. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>Step1 Empathy</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>hey I totally get it, no pressure at all okay?</t>
-        </is>
-      </c>
-      <c r="C5" s="11" t="inlineStr">
-        <is>
-          <t>EMPATHY. Zero judgment. Still engaged -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>ACCEPT. Continue sexting 4-5 msgs before Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1762,7 +1734,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1801,74 +1773,56 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Protect</t>
+          <t>Step3 PWYW</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>it's totally cool, you being here is what matters</t>
+          <t>send me anything, even the smallest amount, I need you to see what you did to me</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>PROTECT. Continue conversation.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>PWYW.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>Step2 Reframe</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>send whatever feels right, even $1... I just can't keep this from you</t>
+          <t>forget about money for a sec... I just want to share this with you, what you're making me feel is real</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>PWYW. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>REFRAME. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Test</t>
+          <t>Step1 Accept</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>what about just [small amount]? I really don't want you to miss this</t>
+          <t>no worries at all, I don't care about that I'm just enjoying this</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>TEST. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>Step1 Empathy</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>that's fine, seriously don't worry about it</t>
-        </is>
-      </c>
-      <c r="C5" s="11" t="inlineStr">
-        <is>
-          <t>EMPATHY. Still engaged -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>ACCEPT. Continue sexting 4-5 msgs before Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1920,56 +1874,56 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>Step3 Urgency</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>just send whatever you want, even $1, I can't keep this to myself... you need to see it</t>
+          <t>figure it out soon man, I'm in this mood rn and I don't know how long it's gonna last</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>PAY WHAT YOU WANT. $1 breaks identity.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>URGENCY.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 Reframe</t>
+          <t>Step2 AltCard</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>look this isn't about money... I just need you to see what you're doing to me rn, I don't react like this to people</t>
+          <t>try a different card? I really don't want you to miss this</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>EMOTIONAL REFRAME. After sexting buildup. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>ALTERNATIVE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Accept</t>
+          <t>Step1 Retry</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>that's totally fine I'm not trying to sell you anything, I just like talking to you</t>
+          <t>ahh that sucks, happens sometimes though try again it usually works the second time</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>ACCEPT. Disarm. THEN: continue sexting 4-5 msgs before Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>RETRY. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2021,56 +1975,56 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>Step3 Urgency</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>send me anything, even the smallest amount, I need you to see what you did to me</t>
+          <t>I want you to see this before I change my mind, I don't keep stuff like this around forever</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>PWYW.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>URGENCY.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 Reframe</t>
+          <t>Step2 AltCard</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>forget about money for a sec... I just want to share this with you, what you're making me feel is real</t>
+          <t>do you have another card you can try? I really want you to see this</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>REFRAME. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>ALTERNATIVE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Accept</t>
+          <t>Step1 Retry</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>no worries at all, I don't care about that I'm just enjoying this</t>
+          <t>damn that's annoying, it happens a lot just try one more time</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>ACCEPT. Disarm. THEN: continue sexting 4-5 msgs before Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>RETRY. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2078,6 +2032,386 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12" t="inlineStr">
+        <is>
+          <t>Step4 Accept</t>
+        </is>
+      </c>
+      <c r="B2" s="12" t="inlineStr">
+        <is>
+          <t>alright I'll chill... for now, no promises though haha</t>
+        </is>
+      </c>
+      <c r="C2" s="12" t="inlineStr">
+        <is>
+          <t>ACCEPT. Door open.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>Step3 ReAttempt</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>look I can't help it, there's something about you that's messing with my head rn</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>RE-ATTEMPT. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>Step2 Subtle</t>
+        </is>
+      </c>
+      <c r="B4" s="12" t="inlineStr">
+        <is>
+          <t>so tell me more about you... what do you do when you're not making dudes on the internet lose their minds?</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>SUBTLE. → Step 3 later.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>Step1 Respect</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>haha alright alright I got a little carried away, you're just too easy to talk to</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>RESPECT. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="12" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="12" t="inlineStr">
+        <is>
+          <t>Step4 Accept</t>
+        </is>
+      </c>
+      <c r="B2" s="12" t="inlineStr">
+        <is>
+          <t>fine I'll stop but don't blame me if it happens again later</t>
+        </is>
+      </c>
+      <c r="C2" s="12" t="inlineStr">
+        <is>
+          <t>ACCEPT.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>Step3 ReAttempt</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>I'm trying to behave but you're making it really hard man, there's something about you</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>RE-ATTEMPT. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>Step2 Subtle</t>
+        </is>
+      </c>
+      <c r="B4" s="12" t="inlineStr">
+        <is>
+          <t>okay new topic, but first... what's the most wild thing you've ever done?</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>SUBTLE. → Step 3 later.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>Step1 Respect</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>my bad I got ahead of myself haha, it's your fault for being so fun to talk to</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>RESPECT. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="12" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>NR-W5</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>can't stop thinking about earlier 😏 you around?</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>2-6 hrs later. New topic.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Character limits
+Name: Up to 64 characters
+Tag: Up to 32 characters
+Text: Up to 1000 characters
+Note: Up to 246 characters
+Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>NR-W4</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>hey hope you're good bro 💪 hit me up when you're back</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>15-30 min later. Warm close.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>NR-W3</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>aight I guess you're busy 😏 might delete this, it was only for you</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>5-10 min later. Takeaway.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>NR-W2</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>you need to see what I just did... seriously 🥵</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>3-5 min later. Curiosity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>NR-W1</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>yo? 🥵</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Send 2-3 min after PPV.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2120,65 +2454,65 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
-        <is>
-          <t>Step3 Urgency</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>figure it out soon man, I'm in this mood rn and I don't know how long it's gonna last</t>
-        </is>
-      </c>
-      <c r="C2" s="11" t="inlineStr">
-        <is>
-          <t>SOFT URGENCY. FOMO.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+      <c r="A2" s="12" t="inlineStr">
+        <is>
+          <t>Step3 Retake</t>
+        </is>
+      </c>
+      <c r="B2" s="12" t="inlineStr">
+        <is>
+          <t>okay wait no I remember now, so like I was saying...</t>
+        </is>
+      </c>
+      <c r="C2" s="12" t="inlineStr">
+        <is>
+          <t>RETAKE. Resume main script.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
-        <is>
-          <t>Step2 AltCard</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>try a different card? I really don't want you to miss this</t>
-        </is>
-      </c>
-      <c r="C3" s="11" t="inlineStr">
-        <is>
-          <t>ALTERNATIVE. Still fails -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>Step2 Redirect</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>but hold on you totally distracted me, I was about to tell you something and now I lost my train of thought...</t>
+        </is>
+      </c>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>REDIRECT. → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="inlineStr">
-        <is>
-          <t>Step1 Retry</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>ahh that sucks, happens sometimes though try again it usually works the second time</t>
-        </is>
-      </c>
-      <c r="C4" s="11" t="inlineStr">
-        <is>
-          <t>RETRY. Normalize. Still fails -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>Step1 Acknowledge</t>
+        </is>
+      </c>
+      <c r="B4" s="12" t="inlineStr">
+        <is>
+          <t>haha wait that's actually funny</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>ACKNOWLEDGE. Adapt. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2221,472 +2555,58 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
-        <is>
-          <t>Step3 Urgency</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>I want you to see this before I change my mind, I don't keep stuff like this around forever</t>
-        </is>
-      </c>
-      <c r="C2" s="11" t="inlineStr">
-        <is>
-          <t>URGENCY.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="inlineStr">
-        <is>
-          <t>Step2 AltCard</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>do you have another card you can try? I really want you to see this</t>
-        </is>
-      </c>
-      <c r="C3" s="11" t="inlineStr">
-        <is>
-          <t>ALTERNATIVE. Still fails -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="11" t="inlineStr">
-        <is>
-          <t>Step1 Retry</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>damn that's annoying, it happens a lot just try one more time</t>
-        </is>
-      </c>
-      <c r="C4" s="11" t="inlineStr">
-        <is>
-          <t>RETRY. Still fails -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="45" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>MR-OBJ-3</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>look I don't do this for just anyone. appreciate what you're getting rn 💪 if that's not your thing it's cool</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>Firm redirect. If still only wants to meet → 'no worries bro 💪 hit me up whenever' and disengage.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Character limits
-Name: Up to 64 characters
-Tag: Up to 32 characters
-Text: Up to 1000 characters
-Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>MR-OBJ-2</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>you really that impatient? 😈 I promise what I'm about to show you is worth it</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>Challenge + tease</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>MR-OBJ-1</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>patience bro 😏 I don't rush. focus on what's right in front of you</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>Deflect + challenge</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="inlineStr">
-        <is>
-          <t>MR-4</t>
-        </is>
-      </c>
-      <c r="B5" s="7" t="inlineStr">
-        <is>
-          <t>yeah? 😏 that's just a taste man</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="inlineStr">
-        <is>
-          <t>Positive → go to R-1. Asks meeting again → MR-OBJ. Silent → NR Waves.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>MR-3</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>what do you think 😏</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>SEND PPV 0 — FREE teaser. Wait for reply.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>MR-2</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>trust me... you're gonna wanna see this 😈</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>WAIT 1-2 MIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="inlineStr">
-        <is>
-          <t>MR-1</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>haha easy man 😏 slow down. let me show you something first</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="inlineStr">
-        <is>
-          <t>DO NOT acknowledge 'meet'. Redirect immediately.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step4 Accept</t>
+          <t>Step3 Retake</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>alright I'll chill... for now, no promises though haha</t>
+          <t>OKAY focus, where was I... oh yeah</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>ACCEPT. Door stays open.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>RETAKE.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step3 ReAttempt</t>
+          <t>Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>look I can't help it, there's something about you that's messing with my head rn</t>
+          <t>wait no stop you're distracting me from what I was gonna say...</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>RE-ATTEMPT. Natural. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>REDIRECT. → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step2 Subtle</t>
+          <t>Step1 Acknowledge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>so tell me more about you... what do you do when you're not making dudes on the internet lose their minds?</t>
+          <t>lol okay that's random but I like it</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>SUBTLE TENSION. Flirt without explicit. -&gt; Step 3 later.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="12" t="inlineStr">
-        <is>
-          <t>Step1 Respect</t>
-        </is>
-      </c>
-      <c r="B5" s="12" t="inlineStr">
-        <is>
-          <t>haha alright alright I got a little carried away, you're just too easy to talk to</t>
-        </is>
-      </c>
-      <c r="C5" s="12" t="inlineStr">
-        <is>
-          <t>RESPECT. Never force. Still no -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="12" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="12" t="inlineStr">
-        <is>
-          <t>Step4 Accept</t>
-        </is>
-      </c>
-      <c r="B2" s="12" t="inlineStr">
-        <is>
-          <t>fine I'll stop but don't blame me if it happens again later</t>
-        </is>
-      </c>
-      <c r="C2" s="12" t="inlineStr">
-        <is>
-          <t>ACCEPT. Door open.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t>Step3 ReAttempt</t>
-        </is>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>I'm trying to behave but you're making it really hard man, there's something about you</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="inlineStr">
-        <is>
-          <t>RE-ATTEMPT. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>Step2 Subtle</t>
-        </is>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>okay new topic, but first... what's the most wild thing you've ever done?</t>
-        </is>
-      </c>
-      <c r="C4" s="12" t="inlineStr">
-        <is>
-          <t>SUBTLE TENSION. -&gt; Step 3 later.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="12" t="inlineStr">
-        <is>
-          <t>Step1 Respect</t>
-        </is>
-      </c>
-      <c r="B5" s="12" t="inlineStr">
-        <is>
-          <t>my bad I got ahead of myself haha, it's your fault for being so fun to talk to</t>
-        </is>
-      </c>
-      <c r="C5" s="12" t="inlineStr">
-        <is>
-          <t>RESPECT. Still no -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D5" s="12" t="n"/>
+          <t>ACKNOWLEDGE. Adapt. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2738,56 +2658,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Retake</t>
+          <t>Step3 Grounding</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>okay wait no I remember now, so like I was saying...</t>
+          <t>I get it there's a lot of fake stuff on here, but you felt something in this convo right? because I did... and that's real</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>RETAKE. Continue with next msg from main journey.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>GROUNDING.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>Step2 Challenge</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>but hold on you totally distracted me, I was about to tell you something and now I lost my train of thought...</t>
+          <t>ask me anything, literally anything about me my life whatever. I'm an open book</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. Curiosity hook. -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Acknowledge</t>
+          <t>Step1 Humor</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>haha wait that's actually funny</t>
+          <t>lol do I sound like a bot to you? beep boop... send $5 for human verification haha I'm kidding</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>ACKNOWLEDGE. Adapt to what he actually said. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>HUMOR. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2839,56 +2759,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Retake</t>
+          <t>Step3 Grounding</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>OKAY focus, where was I... oh yeah</t>
+          <t>I know there's a lot of bots on here but what we've been talking about... that felt real to me. didn't it feel real to you?</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>RETAKE. Resume main script.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>GROUNDING.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>Step2 Challenge</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>wait no stop you're distracting me from what I was gonna say...</t>
+          <t>test me, ask me something only a real person would know. go ahead</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Acknowledge</t>
+          <t>Step1 Humor</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>lol okay that's random but I like it</t>
+          <t>wait you think I'm fake?? that's actually the funniest thing anyone's said to me today</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>ACKNOWLEDGE. Adapt. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>HUMOR. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2940,56 +2860,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Grounding</t>
+          <t>Step3 Firm</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I get it there's a lot of fake stuff on here, but you felt something in this convo right? because I did... and that's real</t>
+          <t>I don't do that on here but what I'm about to show you is better than any call... you'll see</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>GROUNDING. Anchor on emotion.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>FIRM. No calls.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>ask me anything, literally anything about me my life whatever. I'm an open book</t>
+          <t>I have something wayyy better for you though, trust me you'll forget you even asked</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>CHALLENGE. He tests = engaged. Still doubts -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>REDIRECT. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Humor</t>
+          <t>Step1 Dodge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>lol do I sound like a bot to you? beep boop... send $5 for human verification haha I'm kidding</t>
+          <t>haha maybe one day if you earn it but not yet... I'm private about that stuff</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>HUMOR. Disarm. Still doubts -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>DODGE. Max does NOT do calls. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3041,56 +2961,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Grounding</t>
+          <t>Step3 Firm</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I know there's a lot of bots on here but what we've been talking about... that felt real to me. didn't it feel real to you?</t>
+          <t>that's not something I do on here but what I have for you is wayyy better than my voice, trust me</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>GROUNDING.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>FIRM.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>test me, ask me something only a real person would know. go ahead</t>
+          <t>how about instead of a call I show you something that'll blow your mind?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>CHALLENGE. Still doubts -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>REDIRECT. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Humor</t>
+          <t>Step1 Dodge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>wait you think I'm fake?? that's actually the funniest thing anyone's said to me today</t>
+          <t>hmmm maybe but you gotta earn that first haha</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>HUMOR. Still doubts -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>DODGE. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3142,56 +3062,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Firm</t>
+          <t>Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I don't do that on here but what I'm about to show you is better than any call... you'll see</t>
+          <t>trust me you won't regret it, I made this one special</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>FIRM BOUNDARY. Redirect to value.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>CLOSE.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>Step2 Price</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I have something wayyy better for you though, trust me you'll forget you even asked</t>
+          <t>I have exactly what you're thinking of, you're gonna lose it... [price]</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. Still insists -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>PRICE. Set based on content.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Dodge</t>
+          <t>Step1 Tease</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>haha maybe one day if you earn it but not yet... I'm private about that stuff</t>
+          <t>you want that? I might have something... actually I definitely have something</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>DODGE. Door not closed. Still asks -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>TEASE. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3243,56 +3163,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Firm</t>
+          <t>Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>that's not something I do on here but what I have for you is wayyy better than my voice, trust me</t>
+          <t>you're not gonna be able to stop watching this one</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>FIRM.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>CLOSE.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>Step2 Price</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>how about instead of a call I show you something that'll blow your mind?</t>
+          <t>I actually did something just like that, [price] and it's worth every cent</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. Still insists -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>PRICE.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Dodge</t>
+          <t>Step1 Tease</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>hmmm maybe but you gotta earn that first haha</t>
+          <t>oh you have good taste... I think I have exactly what you're looking for</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>DODGE. Still asks -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>TEASE. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3349,7 +3269,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>trust me you won't regret it, I made this one special</t>
+          <t>trust me... I know what you need better than you do</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3357,43 +3277,43 @@
           <t>CLOSE.</t>
         </is>
       </c>
-      <c r="D2" s="12" t="n"/>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Price</t>
+          <t>Step2 Alternative</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I have exactly what you're thinking of, you're gonna lose it... [price]</t>
+          <t>actually what I have might be even crazier and literally no one else has seen it yet</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>PRICE. Set based on content.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>ALTERNATIVE + FOMO. → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Tease</t>
+          <t>Step1 Redirect</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>you want that? I might have something... actually I definitely have something</t>
+          <t>I don't have exactly that but honestly I have something that'll make you forget you even asked</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>TEASE. Build anticipation. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>REDIRECT. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3450,7 +3370,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>you're not gonna be able to stop watching this one</t>
+          <t>just trust me on this one, you'll thank me later</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3458,43 +3378,43 @@
           <t>CLOSE.</t>
         </is>
       </c>
-      <c r="D2" s="12" t="n"/>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Price</t>
+          <t>Step2 Alternative</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I actually did something just like that, [price] and it's worth every cent</t>
+          <t>what I DO have is something no one has ever seen and I think it's even better than what you asked for</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>PRICE.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>ALTERNATIVE. → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Tease</t>
+          <t>Step1 Redirect</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>oh you have good taste... I think I have exactly what you're looking for</t>
+          <t>I don't have that specific thing but I have something you're gonna like even more</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>TEASE. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>REDIRECT. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3507,7 +3427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3544,99 +3464,135 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>NR-W5</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>can't stop thinking about earlier 😏 you around?</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>Send 2-6 hrs later. New convo, don't retry same PPV.</t>
-        </is>
-      </c>
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>I'm 20 but trust me I know what I'm doing 😏</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Character limits
+          <t>Character limits
 Name: Up to 64 characters
 Tag: Up to 32 characters
 Text: Up to 1000 characters
 Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
+Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>NR-W4</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>hey hope you're good bro 💪 hit me up when you're back</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>Send 15-30 min later. Warm close.</t>
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>from Rome originally but I'm in the states now. moved when I was 18</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>NEVER give specific address. Match fan's city if from dating apps.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>NR-W3</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>aight I guess you're busy 😏 might delete this, it was only for you</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>Send 5-10 min later. Takeaway.</t>
-        </is>
-      </c>
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Profession</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>modeling and content creation. also help with my family's business</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>NR-W2</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>you need to see what I just did... seriously 🥵</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>Send 3-5 min later. Curiosity.</t>
-        </is>
-      </c>
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Hobbies</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>gym and boxing is my life bro. 5-6 times a week. that and traveling, fashion, cars 💪</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>NR-W1</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>yo? 🥵</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>Send 2-3 min after PPV. Ping.</t>
-        </is>
-      </c>
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>Countries</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>I've been everywhere... Spain, Dubai, Bali, France, London, Netherlands, Argentina, Brazil</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>Relationship</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>single. I don't do relationships rn... too busy living 😏</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>Favorite</t>
+        </is>
+      </c>
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Italy will always be home but honestly Bali hit different 🌴</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="inlineStr">
+        <is>
+          <t>Tattoos</t>
+        </is>
+      </c>
+      <c r="B9" s="9" t="inlineStr">
+        <is>
+          <t>yeah I got 16 all over. each one has a story 😏</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>black Mustang 🖤</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3688,56 +3644,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>Step3 Seed</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>trust me... I know what you need better than you do</t>
+          <t>okay but next time you have to wait for me, I have something insane planned for round 2</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>CONFIDENCE CLOSE.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Alternative</t>
+          <t>Step2 Rescue</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>actually what I have might be even crazier and literally no one else has seen it yet</t>
+          <t>but I haven't finished yet, don't you wanna watch me cum too?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>ALTERNATIVE + FOMO. -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>RESCUE. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Redirect</t>
+          <t>Step1 Validate</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>I don't have exactly that but honestly I have something that'll make you forget you even asked</t>
+          <t>fuck that's hot, you came because of me??</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>VALIDATE. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3789,56 +3745,56 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>Step3 Seed</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>just trust me on this one, you'll thank me later</t>
+          <t>next time you HAVE to hold it because what I have planned for us next time is way crazier</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>CLOSE.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Alternative</t>
+          <t>Step2 Rescue</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>what I DO have is something no one has ever seen and I think it's even better than what you asked for</t>
+          <t>wait but I'm not done yet, you're gonna leave me like this?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>ALTERNATIVE. -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
+          <t>RESCUE. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D3" s="12" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Redirect</t>
+          <t>Step1 Validate</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>I don't have that specific thing but I have something you're gonna like even more</t>
+          <t>already?? damn that's hot</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
+          <t>VALIDATE. → Step 2.</t>
+        </is>
+      </c>
+      <c r="D4" s="12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3846,208 +3802,6 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="12" t="inlineStr">
-        <is>
-          <t>Step3 Seed</t>
-        </is>
-      </c>
-      <c r="B2" s="12" t="inlineStr">
-        <is>
-          <t>okay but next time you have to wait for me, I have something insane planned for round 2</t>
-        </is>
-      </c>
-      <c r="C2" s="12" t="inlineStr">
-        <is>
-          <t>SEED. Anticipation.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t>Step2 Rescue</t>
-        </is>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>but I haven't finished yet, don't you wanna watch me cum too?</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="inlineStr">
-        <is>
-          <t>RESCUE. Flip to HIM. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>Step1 Validate</t>
-        </is>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>fuck that's hot, you came because of me??</t>
-        </is>
-      </c>
-      <c r="C4" s="12" t="inlineStr">
-        <is>
-          <t>VALIDATE. Feed ego. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="12" t="inlineStr">
-        <is>
-          <t>Step3 Seed</t>
-        </is>
-      </c>
-      <c r="B2" s="12" t="inlineStr">
-        <is>
-          <t>next time you HAVE to hold it because what I have planned for us next time is way crazier</t>
-        </is>
-      </c>
-      <c r="C2" s="12" t="inlineStr">
-        <is>
-          <t>SEED.</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="12" t="inlineStr">
-        <is>
-          <t>Step2 Rescue</t>
-        </is>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>wait but I'm not done yet, you're gonna leave me like this?</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="inlineStr">
-        <is>
-          <t>RESCUE. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D3" s="12" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="12" t="inlineStr">
-        <is>
-          <t>Step1 Validate</t>
-        </is>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>already?? damn that's hot</t>
-        </is>
-      </c>
-      <c r="C4" s="12" t="inlineStr">
-        <is>
-          <t>VALIDATE. -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D4" s="12" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4105,7 +3859,7 @@
           <t>DELAY variant.</t>
         </is>
       </c>
-      <c r="D2" s="13" t="n"/>
+      <c r="D2" s="13" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -4120,10 +3874,10 @@
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>DELAY. Next PPV coming.</t>
-        </is>
-      </c>
-      <c r="D3" s="13" t="n"/>
+          <t>DELAY. Send PPV.</t>
+        </is>
+      </c>
+      <c r="D3" s="13" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -4141,7 +3895,7 @@
           <t>SYNC variant.</t>
         </is>
       </c>
-      <c r="D4" s="13" t="n"/>
+      <c r="D4" s="13" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -4156,10 +3910,10 @@
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>SYNC. Final PPV.</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="n"/>
+          <t>SYNC. Send PPV.</t>
+        </is>
+      </c>
+      <c r="D5" s="13" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
@@ -4177,7 +3931,7 @@
           <t>EDGE variant.</t>
         </is>
       </c>
-      <c r="D6" s="13" t="n"/>
+      <c r="D6" s="13" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
@@ -4192,17 +3946,17 @@
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>EDGE. More PPVs left.</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="n"/>
+          <t>CONTROL.</t>
+        </is>
+      </c>
+      <c r="D7" s="13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4257,10 +4011,10 @@
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>LEVERAGE variant. WAIT 1-2 min.</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="n"/>
+          <t>LEVERAGE variant.</t>
+        </is>
+      </c>
+      <c r="D2" s="13" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -4275,10 +4029,10 @@
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>LEVERAGE. WAIT 1-2 min then send PPV.</t>
-        </is>
-      </c>
-      <c r="D3" s="13" t="n"/>
+          <t>LEVERAGE → WAIT 1-2 min then send PPV.</t>
+        </is>
+      </c>
+      <c r="D3" s="13" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -4296,7 +4050,7 @@
           <t>DURING RAPPORT variant.</t>
         </is>
       </c>
-      <c r="D4" s="13" t="n"/>
+      <c r="D4" s="13" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -4311,10 +4065,10 @@
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>DURING RAPPORT. Fast-track to teasing.</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="n"/>
+          <t>DURING RAPPORT.</t>
+        </is>
+      </c>
+      <c r="D5" s="13" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
@@ -4332,7 +4086,7 @@
           <t>DURING SEXTING variant.</t>
         </is>
       </c>
-      <c r="D6" s="13" t="n"/>
+      <c r="D6" s="13" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
@@ -4347,17 +4101,17 @@
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>DURING SEXTING. React + leverage for PPV.</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="n"/>
+          <t>DURING SEXTING.</t>
+        </is>
+      </c>
+      <c r="D7" s="13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4412,10 +4166,10 @@
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>BOOSTER. Max personality.</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="n"/>
+          <t>BOOSTER. Max personality — gym bro.</t>
+        </is>
+      </c>
+      <c r="D2" s="13" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
@@ -4433,7 +4187,7 @@
           <t>BOOSTER. Ultra micro.</t>
         </is>
       </c>
-      <c r="D3" s="13" t="n"/>
+      <c r="D3" s="13" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -4451,7 +4205,7 @@
           <t>BOOSTER. Physical.</t>
         </is>
       </c>
-      <c r="D4" s="13" t="n"/>
+      <c r="D4" s="13" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
@@ -4469,7 +4223,7 @@
           <t>BOOSTER.</t>
         </is>
       </c>
-      <c r="D5" s="13" t="n"/>
+      <c r="D5" s="13" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
@@ -4487,7 +4241,7 @@
           <t>BOOSTER.</t>
         </is>
       </c>
-      <c r="D6" s="13" t="n"/>
+      <c r="D6" s="13" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
@@ -4505,7 +4259,7 @@
           <t>BOOSTER. Micro.</t>
         </is>
       </c>
-      <c r="D7" s="13" t="n"/>
+      <c r="D7" s="13" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="inlineStr">
@@ -4520,10 +4274,10 @@
       </c>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>BOOSTER. Ego feed.</t>
-        </is>
-      </c>
-      <c r="D8" s="13" t="n"/>
+          <t>BOOSTER. Ego.</t>
+        </is>
+      </c>
+      <c r="D8" s="13" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
@@ -4541,7 +4295,7 @@
           <t>MID-SEXTING BOOSTER.</t>
         </is>
       </c>
-      <c r="D9" s="13" t="n"/>
+      <c r="D9" s="13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4549,184 +4303,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="45" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="9" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B2" s="9" t="inlineStr">
-        <is>
-          <t>I'm 20 but trust me I know what I'm doing 😏</t>
-        </is>
-      </c>
-      <c r="C2" s="9" t="n"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Character limits
-Name: Up to 64 characters
-Tag: Up to 32 characters
-Text: Up to 1000 characters
-Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>from Rome originally but I'm in the states now. moved when I was 18</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>NEVER name a specific US city</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>Profession</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>modeling and content creation. also help with my family's business</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>Hobbies</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>gym and boxing is my life bro. 5-6 times a week. that and traveling, fashion, cars 💪</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>Countries</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>I've been everywhere... Spain, Dubai, Bali, France, London, Netherlands, Argentina, Brazil</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>Relationship</t>
-        </is>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>single. I don't do relationships rn... too busy living 😏</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>Favorite</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="inlineStr">
-        <is>
-          <t>Italy will always be home but honestly Bali hit different 🌴</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>Tattoos</t>
-        </is>
-      </c>
-      <c r="B9" s="9" t="inlineStr">
-        <is>
-          <t>yeah I got 16 all over. each one has a story 😏</t>
-        </is>
-      </c>
-      <c r="C9" s="9" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B10" s="9" t="inlineStr">
-        <is>
-          <t>black Mustang 🖤</t>
-        </is>
-      </c>
-      <c r="C10" s="9" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4779,19 +4355,15 @@
           <t>respect man... I actually prefer guys who know what they want. no games 💪</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
-        <is>
-          <t>He's 40+</t>
-        </is>
-      </c>
+      <c r="C2" s="9" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Character limits
+          <t>Character limits
 Name: Up to 64 characters
 Tag: Up to 32 characters
 Text: Up to 1000 characters
 Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
+Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported.</t>
         </is>
       </c>
     </row>
@@ -4806,11 +4378,7 @@
           <t>oh nice we're around the same age? that's rare on here, most guys are way older 😏</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>He's in his 20s</t>
-        </is>
-      </c>
+      <c r="C3" s="9" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="inlineStr">
@@ -4823,11 +4391,7 @@
           <t>nah bro that's solid. stability is underrated, I respect that 💪</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>He has a boring job</t>
-        </is>
-      </c>
+      <c r="C4" s="9" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
@@ -4840,11 +4404,7 @@
           <t>wait for real?? ok that's actually sick 🔥</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>He has a cool job</t>
-        </is>
-      </c>
+      <c r="C5" s="9" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="inlineStr">
@@ -4857,11 +4417,7 @@
           <t>I can tell 💪 I respect a guy who takes care of himself</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
-        <is>
-          <t>He's fit / goes to the gym</t>
-        </is>
-      </c>
+      <c r="C6" s="9" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="9" t="inlineStr">
@@ -4874,11 +4430,7 @@
           <t>I don't care about that honestly, it's the energy that matters to me 😏</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>He's not fit</t>
-        </is>
-      </c>
+      <c r="C7" s="9" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
@@ -4891,11 +4443,7 @@
           <t>no way 😏 that's crazy</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
-        <is>
-          <t>He says he's in the same city</t>
-        </is>
-      </c>
+      <c r="C8" s="9" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="9" t="inlineStr">
@@ -4908,126 +4456,14 @@
           <t>damn that's far... but distance doesn't matter when the vibe is right 😏</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
-        <is>
-          <t>He's in a different country</t>
-        </is>
-      </c>
+      <c r="C9" s="9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="45" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="9" t="inlineStr">
-        <is>
-          <t>WhereAreYou</t>
-        </is>
-      </c>
-      <c r="B2" s="9" t="inlineStr">
-        <is>
-          <t>I move around a lot man. never in one place for too long 😏</t>
-        </is>
-      </c>
-      <c r="C2" s="9" t="inlineStr">
-        <is>
-          <t>NEVER name a specific location</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Character limits
-Name: Up to 64 characters
-Tag: Up to 32 characters
-Text: Up to 1000 characters
-Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>AreYouIn</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>I travel a lot... I'm all over the place 💪</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>DO NOT confirm or deny any city</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>WhenCanISeeYou</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>haha chill 😏 let me show you something first</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Redirect to MR / content</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5082,17 +4518,17 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>Send next day — seeds next session</t>
+          <t>Next day. Seeds next session.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Character limits
+          <t>Character limits
 Name: Up to 64 characters
 Tag: Up to 32 characters
 Text: Up to 1000 characters
 Note: Up to 246 characters
-Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported. </t>
+Each sheet serves as a tag. Simply replace the sheet name with your desired tag name, and all scripts added to the sheet will be automatically assigned that tag once imported.</t>
         </is>
       </c>
     </row>
@@ -5109,7 +4545,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Send 6-12 hrs after convo goes quiet</t>
+          <t>Send 6-12 hrs after convo goes quiet.</t>
         </is>
       </c>
     </row>
@@ -5118,7 +4554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5173,10 +4609,10 @@
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>SEED. Accept. Continue GFE. Retry later.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
@@ -5191,10 +4627,10 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>DOWNGRADE. Reduce 20-30%. ONE TIME. Still no -&gt; Step 5.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>DOWNGRADE 20-30%. ONE TIME. Still no → Step 5.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
@@ -5209,10 +4645,10 @@
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Ego. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>CHALLENGE. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
@@ -5227,10 +4663,10 @@
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>FOMO. Temporal urgency. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>FOMO. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="11" t="inlineStr">
@@ -5245,17 +4681,17 @@
       </c>
       <c r="C6" s="11" t="inlineStr">
         <is>
-          <t>REFRAME. Compare to cheap item. Wait for response. Still no -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D6" s="11" t="n"/>
+          <t>REFRAME. Still no → Step 2.</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5310,10 +4746,10 @@
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>SEED. Protect relationship.</t>
-        </is>
-      </c>
-      <c r="D2" s="11" t="n"/>
+          <t>SEED.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
@@ -5328,10 +4764,10 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>DOWNGRADE. ONE TIME. Still no -&gt; Step 5.</t>
-        </is>
-      </c>
-      <c r="D3" s="11" t="n"/>
+          <t>DOWNGRADE. ONE TIME. Still no → Step 5.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
@@ -5346,10 +4782,10 @@
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>CHALLENGE. Still no -&gt; Step 4.</t>
-        </is>
-      </c>
-      <c r="D4" s="11" t="n"/>
+          <t>CHALLENGE. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
@@ -5364,10 +4800,10 @@
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>FOMO. Still no -&gt; Step 3.</t>
-        </is>
-      </c>
-      <c r="D5" s="11" t="n"/>
+          <t>FOMO. Still no → Step 3.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="11" t="inlineStr">
@@ -5382,10 +4818,248 @@
       </c>
       <c r="C6" s="11" t="inlineStr">
         <is>
-          <t>REFRAME. Still no -&gt; Step 2.</t>
-        </is>
-      </c>
-      <c r="D6" s="11" t="n"/>
+          <t>REFRAME. Still no → Step 2.</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>Step4 Takeaway</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>if you don't want it that's cool, I'll keep it for myself... or maybe someone else has been asking</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>TAKEAWAY.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t>Step3 Concession</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>alright... [lower price] just for you but don't tell anyone, this stays between us</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>CONCESSION. ONE TIME. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>Step2 Challenge</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>I don't do discounts... I only share this with guys who actually appreciate what they're getting</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Step1 Firmness</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>haha you trying to negotiate with me? this isn't a negotiation man, it's worth every cent</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>FIRMNESS. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>Step4 Takeaway</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>alright I'll save it for someone who actually wants it then</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>TAKEAWAY.</t>
+        </is>
+      </c>
+      <c r="D2" s="11" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t>Step3 Concession</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>fine... [lower price] but ONLY because I like you, one time thing</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>CONCESSION. ONE TIME. Still no → Step 4.</t>
+        </is>
+      </c>
+      <c r="D3" s="11" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>Step2 Challenge</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>the guys who appreciate what I do don't ask for discounts, just saying</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>CHALLENGE. Still → Step 3.</t>
+        </is>
+      </c>
+      <c r="D4" s="11" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Step1 Firmness</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>a discount? do I look like I'm on sale?</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>FIRMNESS. Still → Step 2.</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>